<commit_message>
windturbine producation calculateed per minute and sent to rabbitMq
</commit_message>
<xml_diff>
--- a/regional_simulator/windturbines_mock_data.xlsx
+++ b/regional_simulator/windturbines_mock_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lottediesveld/Documents/Fontys/IntelliJ IDEA/Semester 6/Energy-Grid-Backend/regional_simulator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209578DA-4E5F-1D45-BB84-445E41A3ABCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0B570F-B44A-7A43-9235-1656D2E98EBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,10 +32,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Windsnelheid</t>
+    <t>kW/h</t>
   </si>
   <si>
-    <t>kW/h</t>
+    <t>windspeed</t>
   </si>
 </sst>
 </file>
@@ -297,16 +297,18 @@
   </sheetPr>
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>